<commit_message>
Fixing kirby and additional minor changes (fixing the HUD speed)
</commit_message>
<xml_diff>
--- a/benchmark_report.xlsx
+++ b/benchmark_report.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -43,6 +43,11 @@
         <fgColor rgb="0000CC66"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -56,10 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +452,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>market_data1.csv</t>
+          <t>data/market_data2.csv</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>{'LOT_SIZE': 11, 'HIST_LENGTH': 10, 'delta': 1, 'preferred_lots_low': 9, 'preferred_lots_high': 11, 'margin_adjustment': 0.0005}</t>
+          <t>{'LOT_SIZE': 11, 'HIST_LENGTH': 10, 'delta': 1, 'preferred_lots_low': 8, 'preferred_lots_high': 12, 'margin_adjustment': 0.0005, 'MarketDataFile': 'data/market_data2.csv'}</t>
         </is>
       </c>
     </row>
@@ -519,16 +525,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3915</v>
+        <v>4257</v>
       </c>
       <c r="C3" t="n">
-        <v>4005</v>
+        <v>4354</v>
       </c>
       <c r="D3" t="n">
-        <v>-90</v>
+        <v>-97</v>
       </c>
       <c r="E3" t="n">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F3" t="n">
         <v>134200</v>
@@ -537,13 +543,13 @@
         <v>134300</v>
       </c>
       <c r="H3" t="n">
-        <v>-47412</v>
+        <v>-62791</v>
       </c>
       <c r="I3" t="n">
-        <v>2380366</v>
+        <v>1241491</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>2389366</v>
+        <v>1251191</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -551,119 +557,40 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Match #2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>humming_trader</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>market_data1.csv</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{'LOT_SIZE': 10, 'HIST_LENGTH': 10, 'delta': 1, 'preferred_lots_low': 8, 'preferred_lots_high': 11, 'margin_adjustment': 0.0005}</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BuyVolume</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SellVolume</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EtfPosition</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>FuturePosition</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>EtfPrice</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>FuturePrice</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>TotalFees</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>AccountBalance</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>ProfitOrLoss</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>humming_trader</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>4240</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4323</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-83</v>
-      </c>
-      <c r="E8" t="n">
-        <v>83</v>
-      </c>
-      <c r="F8" t="n">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>optiver_trader</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>6280</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6284</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
         <v>134200</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G4" t="n">
         <v>134300</v>
       </c>
-      <c r="H8" t="n">
-        <v>-56352</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2653990</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>2662290</v>
-      </c>
-      <c r="K8" t="inlineStr">
+      <c r="H4" t="n">
+        <v>94226</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-549426</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>-549026</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>